<commit_message>
Updated UI with initializing button, same data preprocessor class for classifying and training
</commit_message>
<xml_diff>
--- a/models/version 3/model_evaluations.xlsx
+++ b/models/version 3/model_evaluations.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,323 +543,323 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>Extra Trees</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.8095238095238095</v>
+        <v>0.8761904761904762</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.8421052631578947</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.7910447761194029</v>
+        <v>0.8484848484848485</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.8165750196386488</v>
+        <v>0.8857808857808858</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>0.8134141323457897</v>
+        <v>0.8811632811632812</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>0.6956521739130435</v>
+        <v>0.7826086956521739</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>0.8983050847457628</v>
+        <v>0.9491525423728814</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>0.7969786293294031</v>
+        <v>0.8658806190125277</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>0.8095238095238095</v>
+        <v>0.8761904761904762</v>
       </c>
       <c r="K2" s="2" t="n">
-        <v>0.761904761904762</v>
+        <v>0.8470588235294118</v>
       </c>
       <c r="L2" s="2" t="n">
-        <v>0.8412698412698412</v>
+        <v>0.896</v>
       </c>
       <c r="M2" s="2" t="n">
-        <v>0.8015873015873016</v>
+        <v>0.8715294117647059</v>
       </c>
       <c r="N2" s="2" t="n">
-        <v>0.8065003779289492</v>
+        <v>0.8745591036414566</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>SVM</t>
+          <t>Bagging</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.6761904761904762</v>
+        <v>0.8380952380952381</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.7727272727272727</v>
+        <v>0.8372093023255814</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>0.6506024096385542</v>
+        <v>0.8387096774193549</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.7116648411829134</v>
+        <v>0.8379594898724682</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>0.7041047306107546</v>
+        <v>0.8380523702354161</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>0.3695652173913043</v>
+        <v>0.7826086956521739</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>0.9152542372881356</v>
+        <v>0.8813559322033898</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>0.64240972733972</v>
+        <v>0.8319823139277819</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>0.6761904761904762</v>
+        <v>0.8380952380952381</v>
       </c>
       <c r="K3" s="2" t="n">
-        <v>0.4999999999999999</v>
+        <v>0.8089887640449438</v>
       </c>
       <c r="L3" s="2" t="n">
-        <v>0.7605633802816901</v>
+        <v>0.859504132231405</v>
       </c>
       <c r="M3" s="2" t="n">
-        <v>0.630281690140845</v>
+        <v>0.8342464481381744</v>
       </c>
       <c r="N3" s="2" t="n">
-        <v>0.646411804158283</v>
+        <v>0.8373735899782887</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Random Forest</t>
+          <t>KNN</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.8285714285714286</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>0.868421052631579</v>
+        <v>0.8421052631578947</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.8059701492537313</v>
+        <v>0.7910447761194029</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.8371956009426551</v>
+        <v>0.8165750196386488</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.8333295926383122</v>
+        <v>0.8134141323457897</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>0.7173913043478261</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>0.9152542372881356</v>
+        <v>0.8983050847457628</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0.8163227708179808</v>
+        <v>0.7969786293294031</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>0.8285714285714286</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="K4" s="2" t="n">
-        <v>0.7857142857142858</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="L4" s="2" t="n">
-        <v>0.8571428571428572</v>
+        <v>0.8412698412698412</v>
       </c>
       <c r="M4" s="2" t="n">
-        <v>0.8214285714285715</v>
+        <v>0.8015873015873016</v>
       </c>
       <c r="N4" s="2" t="n">
-        <v>0.8258503401360545</v>
+        <v>0.8065003779289492</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Logistic Regression</t>
+          <t>Random Forest</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.7894736842105263</v>
+        <v>0.8611111111111112</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.6395348837209303</v>
+        <v>0.7826086956521739</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.7145042839657283</v>
+        <v>0.8218599033816425</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.7052223582211343</v>
+        <v>0.8170002300437084</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>0.3260869565217391</v>
+        <v>0.6739130434782609</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>0.9322033898305084</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.6291451731761237</v>
+        <v>0.7945836403831983</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="K5" s="2" t="n">
-        <v>0.4615384615384616</v>
+        <v>0.7560975609756099</v>
       </c>
       <c r="L5" s="2" t="n">
-        <v>0.7586206896551724</v>
+        <v>0.8437499999999999</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>0.6100795755968169</v>
+        <v>0.7999237804878049</v>
       </c>
       <c r="N5" s="2" t="n">
-        <v>0.6284703801945181</v>
+        <v>0.8053498838559814</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Decision Tree</t>
+          <t>MLP Classifier</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
         <v>0.8</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0.7906976744186046</v>
+        <v>0.8205128205128205</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>0.8064516129032258</v>
+        <v>0.7878787878787878</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.7985746436609151</v>
+        <v>0.8041958041958042</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>0.7995498874718679</v>
+        <v>0.8021756021756021</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>0.7391304347826086</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>0.847457627118644</v>
+        <v>0.8813559322033898</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>0.7932940309506263</v>
+        <v>0.7885040530582166</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>0.8</v>
       </c>
       <c r="K6" s="2" t="n">
-        <v>0.7640449438202247</v>
+        <v>0.7529411764705882</v>
       </c>
       <c r="L6" s="2" t="n">
-        <v>0.8264462809917354</v>
+        <v>0.832</v>
       </c>
       <c r="M6" s="2" t="n">
-        <v>0.7952456124059801</v>
+        <v>0.792470588235294</v>
       </c>
       <c r="N6" s="2" t="n">
-        <v>0.7991085523261212</v>
+        <v>0.797364705882353</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Naive Bayes</t>
+          <t>Gradient Boosting</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.5904761904761905</v>
+        <v>0.7904761904761904</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.8157894736842105</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.5816326530612245</v>
+        <v>0.7761194029850746</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.6479591836734694</v>
+        <v>0.7959544383346426</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>0.6397473275024296</v>
+        <v>0.7934986720532675</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0.108695652173913</v>
+        <v>0.6739130434782609</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>0.9661016949152542</v>
+        <v>0.8813559322033898</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>0.5373986735445836</v>
+        <v>0.7776344878408253</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>0.5904761904761905</v>
+        <v>0.7904761904761904</v>
       </c>
       <c r="K7" s="2" t="n">
-        <v>0.1886792452830189</v>
+        <v>0.7380952380952381</v>
       </c>
       <c r="L7" s="2" t="n">
-        <v>0.7261146496815286</v>
+        <v>0.8253968253968255</v>
       </c>
       <c r="M7" s="2" t="n">
-        <v>0.4573969474822737</v>
+        <v>0.7817460317460319</v>
       </c>
       <c r="N7" s="2" t="n">
-        <v>0.4906667582307529</v>
+        <v>0.7871504157218444</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Gradient Boosting</t>
+          <t>Decision Tree</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.7904761904761904</v>
+        <v>0.780952380952381</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>0.8157894736842105</v>
+        <v>0.7674418604651163</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.7761194029850746</v>
+        <v>0.7903225806451613</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.7959544383346426</v>
+        <v>0.7788822205551388</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>0.7934986720532675</v>
+        <v>0.7802986460900939</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>0.6739130434782609</v>
+        <v>0.7173913043478261</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>0.8813559322033898</v>
+        <v>0.8305084745762712</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>0.7776344878408253</v>
+        <v>0.7739498894620487</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>0.7904761904761904</v>
+        <v>0.780952380952381</v>
       </c>
       <c r="K8" s="2" t="n">
-        <v>0.7380952380952381</v>
+        <v>0.7415730337078652</v>
       </c>
       <c r="L8" s="2" t="n">
-        <v>0.8253968253968255</v>
+        <v>0.8099173553719008</v>
       </c>
       <c r="M8" s="2" t="n">
-        <v>0.7817460317460319</v>
+        <v>0.775745194539883</v>
       </c>
       <c r="N8" s="2" t="n">
-        <v>0.7871504157218444</v>
+        <v>0.7799760335000375</v>
       </c>
     </row>
     <row r="9">
@@ -911,185 +911,599 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Extra Trees</t>
+          <t>HistGradientBoosting</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.8476190476190476</v>
+        <v>0.7714285714285715</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.8055555555555556</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>0.8115942028985508</v>
+        <v>0.7536231884057971</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.8641304347826086</v>
+        <v>0.7795893719806763</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>0.8576259489302968</v>
+        <v>0.7763745111571199</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>0.7173913043478261</v>
+        <v>0.6304347826086957</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>0.9491525423728814</v>
+        <v>0.8813559322033898</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>0.8332719233603537</v>
+        <v>0.7558953574060427</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0.8476190476190476</v>
+        <v>0.7714285714285715</v>
       </c>
       <c r="K10" s="2" t="n">
-        <v>0.8048780487804877</v>
+        <v>0.7073170731707318</v>
       </c>
       <c r="L10" s="2" t="n">
-        <v>0.8749999999999999</v>
+        <v>0.8124999999999999</v>
       </c>
       <c r="M10" s="2" t="n">
-        <v>0.8399390243902438</v>
+        <v>0.7599085365853658</v>
       </c>
       <c r="N10" s="2" t="n">
-        <v>0.8442799070847851</v>
+        <v>0.7664198606271777</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Linear Discriminant Analysis</t>
+          <t>Quadratic Discriminant Analysis</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.6476190476190476</v>
+        <v>0.7238095238095238</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8148148148148148</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>0.6410256410256411</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.6538461538461539</v>
+        <v>0.7535612535612535</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>0.6522588522588523</v>
+        <v>0.7459774793108127</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0.391304347826087</v>
+        <v>0.4782608695652174</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>0.847457627118644</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>0.6193809874723655</v>
+        <v>0.6967575534266766</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>0.6476190476190476</v>
+        <v>0.7238095238095238</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>0.4931506849315068</v>
+        <v>0.6027397260273973</v>
       </c>
       <c r="L11" s="2" t="n">
-        <v>0.7299270072992702</v>
+        <v>0.7883211678832116</v>
       </c>
       <c r="M11" s="2" t="n">
-        <v>0.6115388461153886</v>
+        <v>0.6955304469553045</v>
       </c>
       <c r="N11" s="2" t="n">
-        <v>0.6261964279762501</v>
+        <v>0.7070188219273311</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>Quadratic Discriminant Analysis</t>
+          <t>Linear SVC</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.7238095238095238</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>0.8148148148148148</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.6923076923076923</v>
+        <v>0.6933333333333334</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.7535612535612535</v>
+        <v>0.73</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>0.7459774793108127</v>
+        <v>0.7254603174603175</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>0.4782608695652174</v>
+        <v>0.5</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>0.9152542372881356</v>
+        <v>0.8813559322033898</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.6967575534266766</v>
+        <v>0.6906779661016949</v>
       </c>
       <c r="J12" s="2" t="n">
-        <v>0.7238095238095238</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="K12" s="2" t="n">
-        <v>0.6027397260273973</v>
+        <v>0.6052631578947369</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0.7883211678832116</v>
+        <v>0.7761194029850748</v>
       </c>
       <c r="M12" s="2" t="n">
-        <v>0.6955304469553045</v>
+        <v>0.6906912804399059</v>
       </c>
       <c r="N12" s="2" t="n">
-        <v>0.7070188219273311</v>
+        <v>0.7012680956121649</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>MLP Classifier</t>
+          <t>Ridge Classifier</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>0.7904761904761904</v>
+        <v>0.6952380952380952</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="D13" s="2" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0.7291666666666666</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>0.7214285714285714</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>0.4130434782608696</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0.9152542372881356</v>
+      </c>
+      <c r="I13" s="2" t="n">
+        <v>0.6641488577745026</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>0.6952380952380952</v>
+      </c>
+      <c r="K13" s="2" t="n">
+        <v>0.5428571428571429</v>
+      </c>
+      <c r="L13" s="2" t="n">
+        <v>0.7714285714285714</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>0.6571428571428571</v>
+      </c>
+      <c r="N13" s="2" t="n">
+        <v>0.6712925170068028</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>SGD Classifier</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>0.6952380952380952</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>0.6590909090909091</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>0.7213114754098361</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.6902011922503726</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>0.6940529415939252</v>
+      </c>
+      <c r="G14" s="2" t="n">
+        <v>0.6304347826086957</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0.7457627118644068</v>
+      </c>
+      <c r="I14" s="2" t="n">
+        <v>0.6880987472365512</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>0.6952380952380952</v>
+      </c>
+      <c r="K14" s="2" t="n">
+        <v>0.6444444444444444</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>0.7333333333333334</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>0.6888888888888889</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>0.6943915343915344</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>Passive Aggressive</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>0.6952380952380952</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0.7692307692307693</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>0.6708860759493671</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0.7200584225900681</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>0.7139704177678861</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>0.4347826086956522</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0.8983050847457628</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>0.6665438467207074</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>0.6952380952380952</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>0.5555555555555555</v>
+      </c>
+      <c r="L15" s="2" t="n">
         <v>0.7681159420289855</v>
       </c>
-      <c r="E13" s="2" t="n">
-        <v>0.8007246376811594</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>0.7966873706004139</v>
-      </c>
-      <c r="G13" s="2" t="n">
-        <v>0.6521739130434783</v>
-      </c>
-      <c r="H13" s="2" t="n">
-        <v>0.8983050847457628</v>
-      </c>
-      <c r="I13" s="2" t="n">
-        <v>0.7752394988946205</v>
-      </c>
-      <c r="J13" s="2" t="n">
-        <v>0.7904761904761904</v>
-      </c>
-      <c r="K13" s="2" t="n">
-        <v>0.7317073170731708</v>
-      </c>
-      <c r="L13" s="2" t="n">
-        <v>0.828125</v>
-      </c>
-      <c r="M13" s="2" t="n">
-        <v>0.7799161585365855</v>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>0.7858848722415795</v>
+      <c r="M15" s="2" t="n">
+        <v>0.6618357487922705</v>
+      </c>
+      <c r="N15" s="2" t="n">
+        <v>0.6749942489072923</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>SVM</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>0.6761904761904762</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>0.7727272727272727</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>0.6506024096385542</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0.7116648411829134</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>0.7041047306107546</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>0.3695652173913043</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>0.9152542372881356</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>0.64240972733972</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>0.6761904761904762</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>0.4999999999999999</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>0.7605633802816901</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>0.630281690140845</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>0.646411804158283</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Logistic Regression</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>0.7894736842105263</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>0.6395348837209303</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0.7145042839657283</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>0.7052223582211343</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>0.3260869565217391</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>0.9322033898305084</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>0.6291451731761237</v>
+      </c>
+      <c r="J17" s="2" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="K17" s="2" t="n">
+        <v>0.4615384615384616</v>
+      </c>
+      <c r="L17" s="2" t="n">
+        <v>0.7586206896551724</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>0.6100795755968169</v>
+      </c>
+      <c r="N17" s="2" t="n">
+        <v>0.6284703801945181</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Linear Discriminant Analysis</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>0.6476190476190476</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>0.6410256410256411</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0.6538461538461539</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>0.6522588522588523</v>
+      </c>
+      <c r="G18" s="2" t="n">
+        <v>0.391304347826087</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>0.847457627118644</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>0.6193809874723655</v>
+      </c>
+      <c r="J18" s="2" t="n">
+        <v>0.6476190476190476</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>0.4931506849315068</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>0.7299270072992702</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>0.6115388461153886</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>0.6261964279762501</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>Ridge Classifier CV</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>0.6476190476190476</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0.7647058823529411</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0.6948529411764706</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>0.6862044817927171</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>0.2826086956521739</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0.9322033898305084</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>0.6074060427413411</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>0.6476190476190476</v>
+      </c>
+      <c r="K19" s="2" t="n">
+        <v>0.4126984126984127</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>0.7482993197278912</v>
+      </c>
+      <c r="M19" s="2" t="n">
+        <v>0.5804988662131519</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>0.6012741604578339</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>Nearest Centroid</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>0.6285714285714286</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0.7058823529411765</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>0.6136363636363636</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0.6597593582887701</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>0.6540488922841865</v>
+      </c>
+      <c r="G20" s="2" t="n">
+        <v>0.2608695652173913</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>0.9152542372881356</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>0.5880619012527635</v>
+      </c>
+      <c r="J20" s="2" t="n">
+        <v>0.6285714285714286</v>
+      </c>
+      <c r="K20" s="2" t="n">
+        <v>0.380952380952381</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>0.7346938775510204</v>
+      </c>
+      <c r="M20" s="2" t="n">
+        <v>0.5578231292517007</v>
+      </c>
+      <c r="N20" s="2" t="n">
+        <v>0.5797214123744736</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>Perceptron</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>0.5535714285714286</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>0.6938775510204082</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0.6237244897959184</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>0.6324101068999027</v>
+      </c>
+      <c r="G21" s="2" t="n">
+        <v>0.6739130434782609</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>0.576271186440678</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>0.6250921149594695</v>
+      </c>
+      <c r="J21" s="2" t="n">
+        <v>0.6190476190476191</v>
+      </c>
+      <c r="K21" s="2" t="n">
+        <v>0.6078431372549019</v>
+      </c>
+      <c r="L21" s="2" t="n">
+        <v>0.6296296296296295</v>
+      </c>
+      <c r="M21" s="2" t="n">
+        <v>0.6187363834422657</v>
+      </c>
+      <c r="N21" s="2" t="n">
+        <v>0.6200850710654632</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Naive Bayes</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>0.5904761904761905</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="D22" s="2" t="n">
+        <v>0.5816326530612245</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0.6479591836734694</v>
+      </c>
+      <c r="F22" s="2" t="n">
+        <v>0.6397473275024296</v>
+      </c>
+      <c r="G22" s="2" t="n">
+        <v>0.108695652173913</v>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>0.9661016949152542</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>0.5373986735445836</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>0.5904761904761905</v>
+      </c>
+      <c r="K22" s="2" t="n">
+        <v>0.1886792452830189</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>0.7261146496815286</v>
+      </c>
+      <c r="M22" s="2" t="n">
+        <v>0.4573969474822737</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>0.4906667582307529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>